<commit_message>
fix: replace package with correct metadata file
</commit_message>
<xml_diff>
--- a/metadata/AEFI/AEFI_TRACKER_V1_DHIS2.34/reference.xlsx
+++ b/metadata/AEFI/AEFI_TRACKER_V1_DHIS2.34/reference.xlsx
@@ -26,7 +26,7 @@
     <sheet name="indicatorTypes" sheetId="21" r:id="rId21"/>
     <sheet name="dashboards" sheetId="22" r:id="rId22"/>
     <sheet name="dashboardItems" sheetId="23" r:id="rId23"/>
-    <sheet name="charts" sheetId="24" r:id="rId24"/>
+    <sheet name="visualizations" sheetId="24" r:id="rId24"/>
     <sheet name="maps" sheetId="25" r:id="rId25"/>
     <sheet name="eventReports" sheetId="26" r:id="rId26"/>
     <sheet name="programNotificationTemplates" sheetId="27" r:id="rId27"/>
@@ -487,7 +487,7 @@
         <v>DHIS2 version</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>DHIS2.33.8-3c90b70</v>
+        <v>DHIS2.34.4-aff07fb</v>
       </c>
     </row>
     <row r="6">
@@ -495,7 +495,7 @@
         <v>Created</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>20210406T115721</v>
+        <v>20210406T141800</v>
       </c>
     </row>
     <row r="7">
@@ -503,7 +503,7 @@
         <v>Identifier</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>AEFI_TRACKER_V1.1.2_DHIS2.33.8-3c90b70_20210406T115721</v>
+        <v>AEFI_TRACKER_V1.1.2_DHIS2.34.4-aff07fb_20210406T141800</v>
       </c>
     </row>
   </sheetData>
@@ -7596,7 +7596,7 @@
         <v>KpmevHebldP</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>Chart</v>
+        <v>SINGLE_VALUE</v>
       </c>
       <c r="C3" s="5" t="str">
         <v>AEFI Deaths</v>
@@ -7616,7 +7616,7 @@
         <v>TjzpPA8uOca</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>Chart</v>
+        <v>SINGLE_VALUE</v>
       </c>
       <c r="C4" s="4" t="str">
         <v>AEFI Hospitalisations</v>
@@ -7633,13 +7633,13 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>lT6Ev0gPL2L</v>
+        <v/>
       </c>
       <c r="B5" s="5" t="str">
-        <v>Map</v>
+        <v>MAP</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>Geographic distribution of AEFI cases</v>
+        <v/>
       </c>
       <c r="D5" s="5" t="str">
         <v>r0sqJrBUsfN</v>
@@ -7656,7 +7656,7 @@
         <v>sODMmX8hJOJ</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>Chart</v>
+        <v>PIE</v>
       </c>
       <c r="C6" s="4" t="str">
         <v>AEFI - Final sub-classification</v>
@@ -7676,7 +7676,7 @@
         <v>j7Bvq96DWgc</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>Chart</v>
+        <v>PIE</v>
       </c>
       <c r="C7" s="5" t="str">
         <v>AEFI - Final classification</v>
@@ -7696,7 +7696,7 @@
         <v>pzX1HTTLJU2</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>Chart</v>
+        <v>SINGLE_VALUE</v>
       </c>
       <c r="C8" s="4" t="str">
         <v>AEFI - Serious cases</v>
@@ -7716,7 +7716,7 @@
         <v>AsmRonHtIuQ</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>Chart</v>
+        <v>SINGLE_VALUE</v>
       </c>
       <c r="C9" s="5" t="str">
         <v>AEFI Cases</v>
@@ -7736,7 +7736,7 @@
         <v>bRZac7ysPZp</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>Chart</v>
+        <v>PIE</v>
       </c>
       <c r="C10" s="4" t="str">
         <v>Autopsy conducted for AEFI-associated deaths</v>
@@ -7756,7 +7756,7 @@
         <v>qeITy0Jv5vV</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>Chart</v>
+        <v>PIE</v>
       </c>
       <c r="C11" s="5" t="str">
         <v>Classification of AEFI cases by Outcome (this year)</v>
@@ -7776,7 +7776,7 @@
         <v>qp7Ml93jnSD</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>Chart</v>
+        <v>PIE</v>
       </c>
       <c r="C12" s="4" t="str">
         <v>Classification of AEFI cases by Seriousness (this year)</v>
@@ -7796,7 +7796,7 @@
         <v>saUrRYwAnKv</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>Chart</v>
+        <v>STACKED_COLUMN</v>
       </c>
       <c r="C13" s="5" t="str">
         <v>AEFI cases considered for Investigation</v>
@@ -7816,7 +7816,7 @@
         <v>ZkbjabzBFJU</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>Chart</v>
+        <v>PIE</v>
       </c>
       <c r="C14" s="4" t="str">
         <v>Annual number of AEFI cases by sex (this year)</v>
@@ -7836,7 +7836,7 @@
         <v>GKTk8X9N0WC</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>Chart</v>
+        <v>PIE</v>
       </c>
       <c r="C15" s="5" t="str">
         <v>Annual number and percentage of AEFI cases by Age (this year)</v>
@@ -7856,7 +7856,7 @@
         <v>fnm8FAWtfX4</v>
       </c>
       <c r="B16" s="4" t="str">
-        <v>Chart</v>
+        <v>PIE</v>
       </c>
       <c r="C16" s="4" t="str">
         <v>AEFI following DPT-Hep B vaccine (this year)</v>
@@ -7876,7 +7876,7 @@
         <v>aGRyKvSt8hB</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>Chart</v>
+        <v>PIE</v>
       </c>
       <c r="C17" s="5" t="str">
         <v>AEFI following PCV vaccine (this year, last year)</v>
@@ -7896,7 +7896,7 @@
         <v>Yjz5dB94OEY</v>
       </c>
       <c r="B18" s="4" t="str">
-        <v>Chart</v>
+        <v>PIE</v>
       </c>
       <c r="C18" s="4" t="str">
         <v>AEFI with IPV (this year)</v>
@@ -7916,7 +7916,7 @@
         <v>LR2jOYXZRms</v>
       </c>
       <c r="B19" s="5" t="str">
-        <v>Chart</v>
+        <v>PIE</v>
       </c>
       <c r="C19" s="5" t="str">
         <v>AEFI following Hepatitis B vaccine (this year)</v>
@@ -7936,7 +7936,7 @@
         <v>wmqeA60KPWU</v>
       </c>
       <c r="B20" s="4" t="str">
-        <v>Chart</v>
+        <v>PIE</v>
       </c>
       <c r="C20" s="4" t="str">
         <v>AEFI with Pentavalent (this year)</v>
@@ -7956,7 +7956,7 @@
         <v>vmnEfVD29Ra</v>
       </c>
       <c r="B21" s="5" t="str">
-        <v>Chart</v>
+        <v>PIE</v>
       </c>
       <c r="C21" s="5" t="str">
         <v>AEFI following Measles,Mumps and Rubella vaccine (this year)</v>
@@ -7976,7 +7976,7 @@
         <v>eVkbnM8lnvP</v>
       </c>
       <c r="B22" s="4" t="str">
-        <v>Chart</v>
+        <v>PIE</v>
       </c>
       <c r="C22" s="4" t="str">
         <v>AEFI following Polio Vaccine - Oral (OPV) Bivalent Types 1 and 3 (this year)</v>
@@ -7996,7 +7996,7 @@
         <v>FzdMlWwP563</v>
       </c>
       <c r="B23" s="5" t="str">
-        <v>Chart</v>
+        <v>PIE</v>
       </c>
       <c r="C23" s="5" t="str">
         <v>AEFI following Rubella vaccine (this year)</v>
@@ -8016,7 +8016,7 @@
         <v>nuw6MOnmL7m</v>
       </c>
       <c r="B24" s="4" t="str">
-        <v>Chart</v>
+        <v>PIE</v>
       </c>
       <c r="C24" s="4" t="str">
         <v>AEFI following BCG 0.05 vaccine (this year)</v>
@@ -8036,7 +8036,7 @@
         <v>EC56gR8oLYB</v>
       </c>
       <c r="B25" s="5" t="str">
-        <v>Chart</v>
+        <v>STACKED_BAR</v>
       </c>
       <c r="C25" s="5" t="str">
         <v>AEFI cases by administered vaccine</v>
@@ -8056,7 +8056,7 @@
         <v>eFP44GxAuby</v>
       </c>
       <c r="B26" s="4" t="str">
-        <v>Chart</v>
+        <v>BAR</v>
       </c>
       <c r="C26" s="4" t="str">
         <v>Types of AEFI reported for all Vaccines (this year)</v>
@@ -8076,7 +8076,7 @@
         <v>phMWM7To0lM</v>
       </c>
       <c r="B27" s="5" t="str">
-        <v>Chart</v>
+        <v>COLUMN</v>
       </c>
       <c r="C27" s="5" t="str">
         <v>Number of AEFI Cases (last 12 months)</v>
@@ -8136,7 +8136,7 @@
         <v>eDFuPQM9v8U</v>
       </c>
       <c r="B30" s="4" t="str">
-        <v>Chart</v>
+        <v>COLUMN</v>
       </c>
       <c r="C30" s="4" t="str">
         <v>AEFI cases following Novavax by Patient's Province and District (this year)</v>
@@ -8156,7 +8156,7 @@
         <v>Gz2dOS3mAiq</v>
       </c>
       <c r="B31" s="5" t="str">
-        <v>Chart</v>
+        <v>COLUMN</v>
       </c>
       <c r="C31" s="5" t="str">
         <v>AEFI cases following Moderna by Patient's Province and District (this year)</v>
@@ -8176,7 +8176,7 @@
         <v>G7B5qhuDM0a</v>
       </c>
       <c r="B32" s="4" t="str">
-        <v>Chart</v>
+        <v>COLUMN</v>
       </c>
       <c r="C32" s="4" t="str">
         <v>AEFI cases following AstraZeneca by Patient's Province and District (this year)</v>
@@ -8196,7 +8196,7 @@
         <v>UnIGdvIWQ1N</v>
       </c>
       <c r="B33" s="5" t="str">
-        <v>Chart</v>
+        <v>COLUMN</v>
       </c>
       <c r="C33" s="5" t="str">
         <v>Adverse events following COVID vaccination by Patient's Province and District</v>
@@ -8213,13 +8213,13 @@
     </row>
     <row r="34">
       <c r="A34" s="4" t="str">
-        <v>qd6vT5pVNlB</v>
+        <v/>
       </c>
       <c r="B34" s="4" t="str">
-        <v>Map</v>
+        <v>MAP</v>
       </c>
       <c r="C34" s="4" t="str">
-        <v>Geographic distribution of Novavax-related AEFI cases</v>
+        <v/>
       </c>
       <c r="D34" s="4" t="str">
         <v>MzvccUOi5xh</v>
@@ -8233,13 +8233,13 @@
     </row>
     <row r="35">
       <c r="A35" s="5" t="str">
-        <v>KCnw54kmHc3</v>
+        <v/>
       </c>
       <c r="B35" s="5" t="str">
-        <v>Map</v>
+        <v>MAP</v>
       </c>
       <c r="C35" s="5" t="str">
-        <v>Geographic distribution of Moderna-related AEFI cases</v>
+        <v/>
       </c>
       <c r="D35" s="5" t="str">
         <v>En9wd6a5rpU</v>
@@ -8253,13 +8253,13 @@
     </row>
     <row r="36">
       <c r="A36" s="4" t="str">
-        <v>zqB888v0wb8</v>
+        <v/>
       </c>
       <c r="B36" s="4" t="str">
-        <v>Map</v>
+        <v>MAP</v>
       </c>
       <c r="C36" s="4" t="str">
-        <v>Geographic distribution of AstraZeneca-related AEFI cases</v>
+        <v/>
       </c>
       <c r="D36" s="4" t="str">
         <v>NHlw3TvqqyA</v>
@@ -8276,7 +8276,7 @@
         <v>S24zyEkZ311</v>
       </c>
       <c r="B37" s="5" t="str">
-        <v>Chart</v>
+        <v>SINGLE_VALUE</v>
       </c>
       <c r="C37" s="5" t="str">
         <v>AstraZeneca-associated reported AEFIs</v>
@@ -8296,7 +8296,7 @@
         <v>C5qirWdKTbh</v>
       </c>
       <c r="B38" s="4" t="str">
-        <v>Chart</v>
+        <v>SINGLE_VALUE</v>
       </c>
       <c r="C38" s="4" t="str">
         <v>Moderna-associated reported AEFIs</v>
@@ -8316,7 +8316,7 @@
         <v>byGIC7C7EdF</v>
       </c>
       <c r="B39" s="5" t="str">
-        <v>Chart</v>
+        <v>SINGLE_VALUE</v>
       </c>
       <c r="C39" s="5" t="str">
         <v>Novavax-associated reported AEFIs</v>
@@ -8336,7 +8336,7 @@
         <v>YtRNCMQS4PY</v>
       </c>
       <c r="B40" s="4" t="str">
-        <v>Chart</v>
+        <v>COLUMN</v>
       </c>
       <c r="C40" s="4" t="str">
         <v>Adverse event following COVID vaccination: AstraZeneca by pregnancy and lactation status</v>
@@ -8356,7 +8356,7 @@
         <v>RXlC5aWvN8v</v>
       </c>
       <c r="B41" s="5" t="str">
-        <v>Chart</v>
+        <v>COLUMN</v>
       </c>
       <c r="C41" s="5" t="str">
         <v>Adverse event following COVID vaccination: Moderna  by pregnancy and lactation status</v>
@@ -8376,7 +8376,7 @@
         <v>P8iSxCvY6AA</v>
       </c>
       <c r="B42" s="4" t="str">
-        <v>Chart</v>
+        <v>COLUMN</v>
       </c>
       <c r="C42" s="4" t="str">
         <v>Adverse event following COVID vaccination: Novavax by pregnancy and lactation status</v>
@@ -8396,7 +8396,7 @@
         <v>L15cr5GjPYB</v>
       </c>
       <c r="B43" s="5" t="str">
-        <v>Chart</v>
+        <v>STACKED_BAR</v>
       </c>
       <c r="C43" s="5" t="str">
         <v>Adverse Events following COVID 19 : Novavax</v>
@@ -8416,7 +8416,7 @@
         <v>Q2fs6GXaHSV</v>
       </c>
       <c r="B44" s="4" t="str">
-        <v>Chart</v>
+        <v>STACKED_BAR</v>
       </c>
       <c r="C44" s="4" t="str">
         <v>Adverse Events following COVID 19 : Moderna</v>
@@ -8436,7 +8436,7 @@
         <v>Lonv4dwIjk4</v>
       </c>
       <c r="B45" s="5" t="str">
-        <v>Chart</v>
+        <v>STACKED_BAR</v>
       </c>
       <c r="C45" s="5" t="str">
         <v>Adverse Events following COVID 19 : AstraZeneca</v>
@@ -8476,7 +8476,7 @@
         <v>NRvH4fN1Uny</v>
       </c>
       <c r="B47" s="5" t="str">
-        <v>Chart</v>
+        <v>PIE</v>
       </c>
       <c r="C47" s="5" t="str">
         <v>Time Interval between Date of Vaccination and Notification to Health System (this year)</v>
@@ -8496,7 +8496,7 @@
         <v>YsgeiuWgtpJ</v>
       </c>
       <c r="B48" s="4" t="str">
-        <v>Chart</v>
+        <v>PIE</v>
       </c>
       <c r="C48" s="4" t="str">
         <v>Time Interval between Reporting by First Level and Date of Notification to Health System (this year)</v>
@@ -8516,7 +8516,7 @@
         <v>I9NvK7o0IUK</v>
       </c>
       <c r="B49" s="5" t="str">
-        <v>Chart</v>
+        <v>PIE</v>
       </c>
       <c r="C49" s="5" t="str">
         <v>Time Interval between Onset and Notification to Health System (this year)</v>
@@ -8536,7 +8536,7 @@
         <v>ARb6cC85Tnr</v>
       </c>
       <c r="B50" s="4" t="str">
-        <v>Chart</v>
+        <v>PIE</v>
       </c>
       <c r="C50" s="4" t="str">
         <v>Time Interval between Date of Notification to Health System and Date of Reporting to National Level</v>
@@ -8587,7 +8587,7 @@
         <v>AEFI Deaths</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C2" s="4" t="str">
         <v/>
@@ -8601,7 +8601,7 @@
         <v>AEFI Hospitalisations</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C3" s="5" t="str">
         <v/>
@@ -8615,7 +8615,7 @@
         <v>AEFI - Final sub-classification</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C4" s="4" t="str">
         <v/>
@@ -8629,7 +8629,7 @@
         <v>AEFI - Final classification</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C5" s="5" t="str">
         <v/>
@@ -8643,7 +8643,7 @@
         <v>AEFI - Serious cases</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C6" s="4" t="str">
         <v/>
@@ -8657,7 +8657,7 @@
         <v>AEFI Cases</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C7" s="5" t="str">
         <v/>
@@ -8671,7 +8671,7 @@
         <v>Autopsy conducted for AEFI-associated deaths</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C8" s="4" t="str">
         <v/>
@@ -8685,7 +8685,7 @@
         <v>Classification of AEFI cases by Outcome (this year)</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C9" s="5" t="str">
         <v/>
@@ -8699,7 +8699,7 @@
         <v>Classification of AEFI cases by Seriousness (this year)</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C10" s="4" t="str">
         <v/>
@@ -8713,7 +8713,7 @@
         <v>AEFI cases considered for Investigation</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C11" s="5" t="str">
         <v/>
@@ -8727,7 +8727,7 @@
         <v>Annual number of AEFI cases by sex (this year)</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C12" s="4" t="str">
         <v/>
@@ -8741,7 +8741,7 @@
         <v>Annual number and percentage of AEFI cases by Age (this year)</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C13" s="5" t="str">
         <v/>
@@ -8755,7 +8755,7 @@
         <v>AEFI following DPT-Hep B vaccine (this year)</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C14" s="4" t="str">
         <v/>
@@ -8769,7 +8769,7 @@
         <v>AEFI following PCV vaccine (this year, last year)</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C15" s="5" t="str">
         <v/>
@@ -8783,7 +8783,7 @@
         <v>AEFI with IPV (this year)</v>
       </c>
       <c r="B16" s="4" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C16" s="4" t="str">
         <v/>
@@ -8797,7 +8797,7 @@
         <v>AEFI following Hepatitis B vaccine (this year)</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C17" s="5" t="str">
         <v/>
@@ -8811,7 +8811,7 @@
         <v>AEFI with Pentavalent (this year)</v>
       </c>
       <c r="B18" s="4" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C18" s="4" t="str">
         <v/>
@@ -8825,7 +8825,7 @@
         <v>AEFI following Measles,Mumps and Rubella vaccine (this year)</v>
       </c>
       <c r="B19" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C19" s="5" t="str">
         <v/>
@@ -8839,7 +8839,7 @@
         <v>AEFI following Polio Vaccine - Oral (OPV) Bivalent Types 1 and 3 (this year)</v>
       </c>
       <c r="B20" s="4" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C20" s="4" t="str">
         <v/>
@@ -8853,7 +8853,7 @@
         <v>AEFI following Rubella vaccine (this year)</v>
       </c>
       <c r="B21" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C21" s="5" t="str">
         <v/>
@@ -8867,7 +8867,7 @@
         <v>AEFI following BCG 0.05 vaccine (this year)</v>
       </c>
       <c r="B22" s="4" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C22" s="4" t="str">
         <v/>
@@ -8881,7 +8881,7 @@
         <v>AEFI cases by administered vaccine</v>
       </c>
       <c r="B23" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C23" s="5" t="str">
         <v/>
@@ -8895,7 +8895,7 @@
         <v>Types of AEFI reported for all Vaccines (this year)</v>
       </c>
       <c r="B24" s="4" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C24" s="4" t="str">
         <v/>
@@ -8909,7 +8909,7 @@
         <v>Number of AEFI Cases (last 12 months)</v>
       </c>
       <c r="B25" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C25" s="5" t="str">
         <v/>
@@ -8923,7 +8923,7 @@
         <v>AEFI cases following Novavax by Patient's Province and District (this year)</v>
       </c>
       <c r="B26" s="4" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C26" s="4" t="str">
         <v/>
@@ -8937,7 +8937,7 @@
         <v>AEFI cases following Moderna by Patient's Province and District (this year)</v>
       </c>
       <c r="B27" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C27" s="5" t="str">
         <v/>
@@ -8951,7 +8951,7 @@
         <v>AEFI cases following AstraZeneca by Patient's Province and District (this year)</v>
       </c>
       <c r="B28" s="4" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C28" s="4" t="str">
         <v/>
@@ -8979,7 +8979,7 @@
         <v>AstraZeneca-associated reported AEFIs</v>
       </c>
       <c r="B30" s="4" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C30" s="4" t="str">
         <v/>
@@ -8993,7 +8993,7 @@
         <v>Moderna-associated reported AEFIs</v>
       </c>
       <c r="B31" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C31" s="5" t="str">
         <v/>
@@ -9007,7 +9007,7 @@
         <v>Novavax-associated reported AEFIs</v>
       </c>
       <c r="B32" s="4" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C32" s="4" t="str">
         <v/>
@@ -9063,7 +9063,7 @@
         <v>Adverse Events following COVID 19 : Novavax</v>
       </c>
       <c r="B36" s="4" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C36" s="4" t="str">
         <v/>
@@ -9077,7 +9077,7 @@
         <v>Adverse Events following COVID 19 : Moderna</v>
       </c>
       <c r="B37" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C37" s="5" t="str">
         <v/>
@@ -9091,7 +9091,7 @@
         <v>Adverse Events following COVID 19 : AstraZeneca</v>
       </c>
       <c r="B38" s="4" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C38" s="4" t="str">
         <v/>
@@ -9105,7 +9105,7 @@
         <v>Time Interval between Date of Vaccination and Notification to Health System (this year)</v>
       </c>
       <c r="B39" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C39" s="5" t="str">
         <v/>
@@ -9119,7 +9119,7 @@
         <v>Time Interval between Reporting by First Level and Date of Notification to Health System (this year)</v>
       </c>
       <c r="B40" s="4" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C40" s="4" t="str">
         <v/>
@@ -9133,7 +9133,7 @@
         <v>Time Interval between Onset and Notification to Health System (this year)</v>
       </c>
       <c r="B41" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C41" s="5" t="str">
         <v/>
@@ -9147,7 +9147,7 @@
         <v>Time Interval between Date of Notification to Health System and Date of Reporting to National Level</v>
       </c>
       <c r="B42" s="4" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C42" s="4" t="str">
         <v/>
@@ -9803,7 +9803,7 @@
         <v>Person</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2021-03-19</v>
+        <v>2021-04-06</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>EZkN8vYZwjR</v>

</xml_diff>